<commit_message>
modificacion columna m y cambios en alcampo
se modifica la formula de la columna M y Se divide el alcampo en dos tipos, y se modifican los porcentajes de sus codigos correspondientes
ALCAMPO FRESCO
- 460 =  28,5% --> 0%
- 6000 = 28,5% --> 0%
- 6001 = 28,5% --> 0%
- 6005 = 28,5% --> 0%

- 459 = 28,5% --> 26,5%
- 461 = 28,5% --> 26,5%

ALCAMPO CONGELADO
- 457 = 28,5% (se mantiene igual)
- 455 = 28,5% (se mantiene igual)
- 6006 = 28,5% (se mantiene igual)
- 6007 = 28,5% (se mantiene igual)
</commit_message>
<xml_diff>
--- a/Cargas Diarias/Cargas Diarias.xlsx
+++ b/Cargas Diarias/Cargas Diarias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\puesto 17\Desktop\Github\Partes\Cargas Diarias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99ADAFF4-9A6A-41D9-97E4-4E134D0E879B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC7AC0A-9A8E-4E5D-A6AE-52F1FCEF1805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCD83F86-A6AF-4FE0-AF75-50E1C7367F1C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="222">
   <si>
     <t xml:space="preserve">DIA  CARGA </t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>ALCALA HENARES</t>
-  </si>
-  <si>
-    <t>ALCAMPO</t>
   </si>
   <si>
     <t>EUGENIO</t>
@@ -701,6 +698,12 @@
   </si>
   <si>
     <t>PANIFICADORA ERELU</t>
+  </si>
+  <si>
+    <t>ALCAMPO CONGELADO</t>
+  </si>
+  <si>
+    <t>ALCAMPO FRESCO</t>
   </si>
 </sst>
 </file>
@@ -1668,7 +1671,7 @@
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5703125" defaultRowHeight="42.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1692,7 +1695,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1719,7 +1722,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1786,7 +1789,7 @@
         <v/>
       </c>
       <c r="L2" s="7" t="str">
-        <f>IF(F2="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f>IF(F2="ALCAMPO CONGELADO ZARAGOZA",IF(I2&lt;27,22.04,""),"")</f>
         <v/>
       </c>
       <c r="M2" s="7" t="str">
@@ -1850,7 +1853,7 @@
         <v/>
       </c>
       <c r="L3" s="7" t="str">
-        <f>IF(F3="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f t="shared" ref="L3:L66" si="4">IF(F3="ALCAMPO CONGELADO ZARAGOZA",IF(I3&lt;27,22.04,""),"")</f>
         <v/>
       </c>
       <c r="M3" s="7" t="str">
@@ -1914,7 +1917,7 @@
         <v/>
       </c>
       <c r="L4" s="7" t="str">
-        <f t="shared" ref="L4:L67" si="4">IF(F4="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M4" s="7" t="str">
@@ -5947,7 +5950,7 @@
         <v/>
       </c>
       <c r="L67" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="L67:L130" si="14">IF(F67="ALCAMPO CONGELADO ZARAGOZA",IF(I67&lt;27,22.04,""),"")</f>
         <v/>
       </c>
       <c r="M67" s="7" t="str">
@@ -6011,7 +6014,7 @@
         <v/>
       </c>
       <c r="L68" s="7" t="str">
-        <f t="shared" ref="L68:L131" si="14">IF(F68="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f t="shared" si="14"/>
         <v/>
       </c>
       <c r="M68" s="7" t="str">
@@ -10043,7 +10046,7 @@
         <v/>
       </c>
       <c r="L131" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="L131:L194" si="24">IF(F131="ALCAMPO CONGELADO ZARAGOZA",IF(I131&lt;27,22.04,""),"")</f>
         <v/>
       </c>
       <c r="M131" s="7" t="str">
@@ -10107,7 +10110,7 @@
         <v/>
       </c>
       <c r="L132" s="7" t="str">
-        <f t="shared" ref="L132:L195" si="24">IF(F132="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f t="shared" si="24"/>
         <v/>
       </c>
       <c r="M132" s="7" t="str">
@@ -14139,7 +14142,7 @@
         <v/>
       </c>
       <c r="L195" s="7" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="L195:L258" si="34">IF(F195="ALCAMPO CONGELADO ZARAGOZA",IF(I195&lt;27,22.04,""),"")</f>
         <v/>
       </c>
       <c r="M195" s="7" t="str">
@@ -14203,7 +14206,7 @@
         <v/>
       </c>
       <c r="L196" s="7" t="str">
-        <f t="shared" ref="L196:L259" si="34">IF(F196="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f t="shared" si="34"/>
         <v/>
       </c>
       <c r="M196" s="7" t="str">
@@ -18235,7 +18238,7 @@
         <v/>
       </c>
       <c r="L259" s="7" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="L259:L322" si="44">IF(F259="ALCAMPO CONGELADO ZARAGOZA",IF(I259&lt;27,22.04,""),"")</f>
         <v/>
       </c>
       <c r="M259" s="7" t="str">
@@ -18299,7 +18302,7 @@
         <v/>
       </c>
       <c r="L260" s="7" t="str">
-        <f t="shared" ref="L260:L323" si="44">IF(F260="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f t="shared" si="44"/>
         <v/>
       </c>
       <c r="M260" s="7" t="str">
@@ -22331,7 +22334,7 @@
         <v/>
       </c>
       <c r="L323" s="7" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" ref="L323:L386" si="53">IF(F323="ALCAMPO CONGELADO ZARAGOZA",IF(I323&lt;27,22.04,""),"")</f>
         <v/>
       </c>
       <c r="M323" s="7" t="str">
@@ -22395,7 +22398,7 @@
         <v/>
       </c>
       <c r="L324" s="7" t="str">
-        <f t="shared" ref="L324:L387" si="53">IF(F324="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f t="shared" si="53"/>
         <v/>
       </c>
       <c r="M324" s="7" t="str">
@@ -26427,7 +26430,7 @@
         <v/>
       </c>
       <c r="L387" s="7" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="L387:L450" si="62">IF(F387="ALCAMPO CONGELADO ZARAGOZA",IF(I387&lt;27,22.04,""),"")</f>
         <v/>
       </c>
       <c r="M387" s="7" t="str">
@@ -26491,7 +26494,7 @@
         <v/>
       </c>
       <c r="L388" s="7" t="str">
-        <f t="shared" ref="L388:L451" si="62">IF(F388="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f t="shared" si="62"/>
         <v/>
       </c>
       <c r="M388" s="7" t="str">
@@ -30523,7 +30526,7 @@
         <v/>
       </c>
       <c r="L451" s="7" t="str">
-        <f t="shared" si="62"/>
+        <f t="shared" ref="L451:L488" si="71">IF(F451="ALCAMPO CONGELADO ZARAGOZA",IF(I451&lt;27,22.04,""),"")</f>
         <v/>
       </c>
       <c r="M451" s="7" t="str">
@@ -30587,7 +30590,7 @@
         <v/>
       </c>
       <c r="L452" s="7" t="str">
-        <f t="shared" ref="L452:L488" si="71">IF(F452="ALCAMPO CONGELADO ZARAGOZA",22.04,"")</f>
+        <f t="shared" si="71"/>
         <v/>
       </c>
       <c r="M452" s="7" t="str">
@@ -32955,10 +32958,10 @@
       </c>
       <c r="J1047488" s="49"/>
       <c r="L1047488" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="M1047488" s="27" t="s">
         <v>191</v>
-      </c>
-      <c r="M1047488" s="27" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="1047489" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -32981,11 +32984,11 @@
         <v>0.28499999999999998</v>
       </c>
       <c r="I1047489" s="16" t="s">
-        <v>33</v>
+        <v>220</v>
       </c>
       <c r="J1047489" s="49"/>
       <c r="L1047489" s="28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M1047489" s="29">
         <v>400</v>
@@ -32993,7 +32996,7 @@
     </row>
     <row r="1047490" spans="2:13" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1047490" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C1047490" s="42">
         <v>0</v>
@@ -33002,20 +33005,20 @@
         <v>457</v>
       </c>
       <c r="F1047490" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1047490" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="G1047490" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="H1047490" s="18">
         <v>0.28499999999999998</v>
       </c>
       <c r="I1047490" s="19" t="s">
-        <v>33</v>
+        <v>220</v>
       </c>
       <c r="J1047490" s="49"/>
       <c r="L1047490" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M1047490" s="31">
         <v>300</v>
@@ -33032,20 +33035,20 @@
         <v>6006</v>
       </c>
       <c r="F1047491" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1047491" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="G1047491" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="H1047491" s="18">
         <v>0.28499999999999998</v>
       </c>
       <c r="I1047491" s="19" t="s">
-        <v>33</v>
+        <v>220</v>
       </c>
       <c r="J1047491" s="49"/>
       <c r="L1047491" s="32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M1047491" s="33">
         <v>350</v>
@@ -33053,7 +33056,7 @@
     </row>
     <row r="1047492" spans="2:13" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1047492" s="41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C1047492" s="42">
         <v>0</v>
@@ -33062,20 +33065,20 @@
         <v>6007</v>
       </c>
       <c r="F1047492" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1047492" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H1047492" s="18">
         <v>0.28499999999999998</v>
       </c>
       <c r="I1047492" s="19" t="s">
-        <v>33</v>
+        <v>220</v>
       </c>
       <c r="J1047492" s="49"/>
       <c r="L1047492" s="32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M1047492" s="33">
         <v>250</v>
@@ -33083,7 +33086,7 @@
     </row>
     <row r="1047493" spans="2:13" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1047493" s="41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1047493" s="42">
         <v>0</v>
@@ -33092,20 +33095,20 @@
         <v>459</v>
       </c>
       <c r="F1047493" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1047493" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1047493" s="18">
-        <v>0.28499999999999998</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="I1047493" s="19" t="s">
-        <v>33</v>
+        <v>221</v>
       </c>
       <c r="J1047493" s="49"/>
       <c r="L1047493" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M1047493" s="33">
         <v>700</v>
@@ -33113,7 +33116,7 @@
     </row>
     <row r="1047494" spans="2:13" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1047494" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1047494" s="42">
         <v>0</v>
@@ -33122,20 +33125,20 @@
         <v>460</v>
       </c>
       <c r="F1047494" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1047494" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1047494" s="18">
-        <v>0.28499999999999998</v>
+        <v>0</v>
       </c>
       <c r="I1047494" s="19" t="s">
-        <v>33</v>
+        <v>221</v>
       </c>
       <c r="J1047494" s="49"/>
       <c r="L1047494" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M1047494" s="34">
         <v>200</v>
@@ -33143,7 +33146,7 @@
     </row>
     <row r="1047495" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1047495" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1047495" s="42">
         <v>0</v>
@@ -33152,22 +33155,22 @@
         <v>461</v>
       </c>
       <c r="F1047495" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G1047495" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1047495" s="18">
-        <v>0.28499999999999998</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="I1047495" s="19" t="s">
-        <v>33</v>
+        <v>221</v>
       </c>
       <c r="J1047495" s="49"/>
     </row>
     <row r="1047496" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1047496" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1047496" s="42">
         <v>0</v>
@@ -33176,16 +33179,16 @@
         <v>6000</v>
       </c>
       <c r="F1047496" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1047496" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H1047496" s="18">
-        <v>0.28499999999999998</v>
+        <v>0</v>
       </c>
       <c r="I1047496" s="19" t="s">
-        <v>33</v>
+        <v>221</v>
       </c>
       <c r="J1047496" s="49"/>
     </row>
@@ -33200,16 +33203,16 @@
         <v>6001</v>
       </c>
       <c r="F1047497" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1047497" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="G1047497" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="H1047497" s="18">
-        <v>0.28499999999999998</v>
+        <v>0</v>
       </c>
       <c r="I1047497" s="19" t="s">
-        <v>33</v>
+        <v>221</v>
       </c>
       <c r="J1047497" s="49"/>
     </row>
@@ -33224,16 +33227,16 @@
         <v>6005</v>
       </c>
       <c r="F1047498" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1047498" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1047498" s="18">
-        <v>0.28499999999999998</v>
+        <v>0</v>
       </c>
       <c r="I1047498" s="19" t="s">
-        <v>33</v>
+        <v>221</v>
       </c>
       <c r="J1047498" s="49"/>
     </row>
@@ -33248,10 +33251,10 @@
         <v>12</v>
       </c>
       <c r="F1047499" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1047499" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="G1047499" s="5" t="s">
-        <v>50</v>
       </c>
       <c r="H1047499" s="18"/>
       <c r="I1047499" s="19"/>
@@ -33259,7 +33262,7 @@
     </row>
     <row r="1047500" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1047500" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1047500" s="42">
         <v>0.12</v>
@@ -33268,10 +33271,10 @@
         <v>410</v>
       </c>
       <c r="F1047500" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1047500" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1047500" s="18"/>
       <c r="I1047500" s="19"/>
@@ -33288,10 +33291,10 @@
         <v>109</v>
       </c>
       <c r="F1047501" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1047501" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="G1047501" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="H1047501" s="18"/>
       <c r="I1047501" s="19"/>
@@ -33308,10 +33311,10 @@
         <v>176</v>
       </c>
       <c r="F1047502" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1047502" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="G1047502" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="H1047502" s="18"/>
       <c r="I1047502" s="19"/>
@@ -33319,7 +33322,7 @@
     </row>
     <row r="1047503" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1047503" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1047503" s="42">
         <v>0</v>
@@ -33328,10 +33331,10 @@
         <v>305</v>
       </c>
       <c r="F1047503" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1047503" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="G1047503" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="H1047503" s="18"/>
       <c r="I1047503" s="19"/>
@@ -33339,7 +33342,7 @@
     </row>
     <row r="1047504" spans="2:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1047504" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1047504" s="42">
         <v>0</v>
@@ -33348,10 +33351,10 @@
         <v>57</v>
       </c>
       <c r="F1047504" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1047504" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="G1047504" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="H1047504" s="18"/>
       <c r="I1047504" s="19"/>
@@ -33359,7 +33362,7 @@
     </row>
     <row r="1047505" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1047505" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C1047505" s="42">
         <v>0</v>
@@ -33368,10 +33371,10 @@
         <v>300</v>
       </c>
       <c r="F1047505" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1047505" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="G1047505" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H1047505" s="18"/>
       <c r="I1047505" s="19"/>
@@ -33379,7 +33382,7 @@
     </row>
     <row r="1047506" spans="2:10" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1047506" s="41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C1047506" s="42">
         <v>0.23</v>
@@ -33388,22 +33391,22 @@
         <v>20496</v>
       </c>
       <c r="F1047506" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1047506" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="G1047506" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="H1047506" s="18">
         <v>0.28999999999999998</v>
       </c>
       <c r="I1047506" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J1047506" s="49"/>
     </row>
     <row r="1047507" spans="2:10" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1047507" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C1047507" s="43">
         <v>0</v>
@@ -33412,16 +33415,16 @@
         <v>20492</v>
       </c>
       <c r="F1047507" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1047507" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="G1047507" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="H1047507" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047507" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047507" s="49"/>
     </row>
@@ -33430,16 +33433,16 @@
         <v>20491</v>
       </c>
       <c r="F1047508" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1047508" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="G1047508" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="H1047508" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047508" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047508" s="49"/>
     </row>
@@ -33448,16 +33451,16 @@
         <v>20485</v>
       </c>
       <c r="F1047509" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G1047509" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1047509" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047509" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047509" s="49"/>
     </row>
@@ -33466,16 +33469,16 @@
         <v>20487</v>
       </c>
       <c r="F1047510" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G1047510" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1047510" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047510" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047510" s="49"/>
     </row>
@@ -33484,16 +33487,16 @@
         <v>20486</v>
       </c>
       <c r="F1047511" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1047511" s="5" t="s">
         <v>75</v>
-      </c>
-      <c r="G1047511" s="5" t="s">
-        <v>76</v>
       </c>
       <c r="H1047511" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047511" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047511" s="49"/>
     </row>
@@ -33502,16 +33505,16 @@
         <v>20488</v>
       </c>
       <c r="F1047512" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G1047512" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H1047512" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047512" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047512" s="49"/>
     </row>
@@ -33520,16 +33523,16 @@
         <v>20490</v>
       </c>
       <c r="F1047513" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1047513" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="G1047513" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="H1047513" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047513" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047513" s="49"/>
     </row>
@@ -33538,16 +33541,16 @@
         <v>20497</v>
       </c>
       <c r="F1047514" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G1047514" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1047514" s="18">
         <v>0.28999999999999998</v>
       </c>
       <c r="I1047514" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J1047514" s="49"/>
     </row>
@@ -33556,16 +33559,16 @@
         <v>20499</v>
       </c>
       <c r="F1047515" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1047515" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="G1047515" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="H1047515" s="18">
         <v>0.28999999999999998</v>
       </c>
       <c r="I1047515" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J1047515" s="49"/>
     </row>
@@ -33574,16 +33577,16 @@
         <v>20489</v>
       </c>
       <c r="F1047516" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G1047516" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1047516" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047516" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047516" s="49"/>
     </row>
@@ -33592,16 +33595,16 @@
         <v>20493</v>
       </c>
       <c r="F1047517" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G1047517" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1047517" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047517" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047517" s="49"/>
     </row>
@@ -33610,16 +33613,16 @@
         <v>20494</v>
       </c>
       <c r="F1047518" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G1047518" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H1047518" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047518" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J1047518" s="49"/>
     </row>
@@ -33628,16 +33631,16 @@
         <v>20495</v>
       </c>
       <c r="F1047519" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1047519" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="G1047519" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="H1047519" s="18">
         <v>0.27039999999999997</v>
       </c>
       <c r="I1047519" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J1047519" s="49"/>
     </row>
@@ -33646,16 +33649,16 @@
         <v>20498</v>
       </c>
       <c r="F1047520" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1047520" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="G1047520" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="H1047520" s="18">
         <v>0.28999999999999998</v>
       </c>
       <c r="I1047520" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J1047520" s="49"/>
     </row>
@@ -33664,16 +33667,16 @@
         <v>408</v>
       </c>
       <c r="F1047521" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1047521" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="G1047521" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="H1047521" s="18">
         <v>0.01</v>
       </c>
       <c r="I1047521" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047521" s="49"/>
     </row>
@@ -33682,16 +33685,16 @@
         <v>406</v>
       </c>
       <c r="F1047522" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1047522" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="G1047522" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="H1047522" s="18">
         <v>0.01</v>
       </c>
       <c r="I1047522" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047522" s="49"/>
     </row>
@@ -33700,10 +33703,10 @@
         <v>206</v>
       </c>
       <c r="F1047523" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1047523" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="G1047523" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="H1047523" s="18"/>
       <c r="I1047523" s="19"/>
@@ -33714,10 +33717,10 @@
         <v>127</v>
       </c>
       <c r="F1047524" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G1047524" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H1047524" s="18"/>
       <c r="I1047524" s="19"/>
@@ -33728,10 +33731,10 @@
         <v>207</v>
       </c>
       <c r="F1047525" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G1047525" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1047525" s="18"/>
       <c r="I1047525" s="19"/>
@@ -33742,10 +33745,10 @@
         <v>503</v>
       </c>
       <c r="F1047526" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1047526" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="G1047526" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="H1047526" s="18"/>
       <c r="I1047526" s="19"/>
@@ -33756,10 +33759,10 @@
         <v>256</v>
       </c>
       <c r="F1047527" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1047527" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="G1047527" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="H1047527" s="18"/>
       <c r="I1047527" s="19"/>
@@ -33770,16 +33773,16 @@
         <v>3</v>
       </c>
       <c r="F1047528" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1047528" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="G1047528" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="H1047528" s="18">
         <v>3.85E-2</v>
       </c>
       <c r="I1047528" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047528" s="49"/>
     </row>
@@ -33788,16 +33791,16 @@
         <v>9058</v>
       </c>
       <c r="F1047529" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1047529" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="G1047529" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="H1047529" s="18">
         <v>6.7699999999999996E-2</v>
       </c>
       <c r="I1047529" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047529" s="49"/>
     </row>
@@ -33806,10 +33809,10 @@
         <v>507</v>
       </c>
       <c r="F1047530" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1047530" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="G1047530" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="H1047530" s="18"/>
       <c r="I1047530" s="19"/>
@@ -33820,10 +33823,10 @@
         <v>1540</v>
       </c>
       <c r="F1047531" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1047531" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="G1047531" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="H1047531" s="18"/>
       <c r="I1047531" s="19"/>
@@ -33834,10 +33837,10 @@
         <v>1575</v>
       </c>
       <c r="F1047532" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G1047532" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H1047532" s="18"/>
       <c r="I1047532" s="19"/>
@@ -33848,10 +33851,10 @@
         <v>1608</v>
       </c>
       <c r="F1047533" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1047533" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="G1047533" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="H1047533" s="18"/>
       <c r="I1047533" s="19"/>
@@ -33862,16 +33865,16 @@
         <v>21055</v>
       </c>
       <c r="F1047534" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1047534" s="5" t="s">
         <v>110</v>
-      </c>
-      <c r="G1047534" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="H1047534" s="18">
         <v>0.28999999999999998</v>
       </c>
       <c r="I1047534" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047534" s="49"/>
     </row>
@@ -33880,16 +33883,16 @@
         <v>21142</v>
       </c>
       <c r="F1047535" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G1047535" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H1047535" s="18">
         <v>0.28999999999999998</v>
       </c>
       <c r="I1047535" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047535" s="49"/>
     </row>
@@ -33898,10 +33901,10 @@
         <v>1646</v>
       </c>
       <c r="F1047536" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G1047536" s="5" t="s">
         <v>113</v>
-      </c>
-      <c r="G1047536" s="5" t="s">
-        <v>114</v>
       </c>
       <c r="H1047536" s="18"/>
       <c r="I1047536" s="19"/>
@@ -33912,10 +33915,10 @@
         <v>185</v>
       </c>
       <c r="F1047537" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1047537" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="G1047537" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="H1047537" s="18"/>
       <c r="I1047537" s="19"/>
@@ -33926,16 +33929,16 @@
         <v>197</v>
       </c>
       <c r="F1047538" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G1047538" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H1047538" s="18">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="I1047538" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047538" s="49"/>
     </row>
@@ -33944,10 +33947,10 @@
         <v>409</v>
       </c>
       <c r="F1047539" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G1047539" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1047539" s="18"/>
       <c r="I1047539" s="19"/>
@@ -33958,10 +33961,10 @@
         <v>513</v>
       </c>
       <c r="F1047540" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G1047540" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1047540" s="18"/>
       <c r="I1047540" s="19"/>
@@ -33972,16 +33975,16 @@
         <v>9063</v>
       </c>
       <c r="F1047541" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G1047541" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1047541" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="I1047541" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047541" s="49"/>
     </row>
@@ -33990,10 +33993,10 @@
         <v>9067</v>
       </c>
       <c r="F1047542" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1047542" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="G1047542" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="H1047542" s="18"/>
       <c r="I1047542" s="19"/>
@@ -34004,10 +34007,10 @@
         <v>9065</v>
       </c>
       <c r="F1047543" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G1047543" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="G1047543" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="H1047543" s="18"/>
       <c r="I1047543" s="19"/>
@@ -34018,10 +34021,10 @@
         <v>98</v>
       </c>
       <c r="F1047544" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1047544" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="G1047544" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="H1047544" s="18"/>
       <c r="I1047544" s="19"/>
@@ -34032,10 +34035,10 @@
         <v>2</v>
       </c>
       <c r="F1047545" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G1047545" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1047545" s="18"/>
       <c r="I1047545" s="19"/>
@@ -34046,10 +34049,10 @@
         <v>9072</v>
       </c>
       <c r="F1047546" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G1047546" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1047546" s="18"/>
       <c r="I1047546" s="19"/>
@@ -34060,10 +34063,10 @@
         <v>7</v>
       </c>
       <c r="F1047547" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G1047547" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1047547" s="18"/>
       <c r="I1047547" s="19"/>
@@ -34074,16 +34077,16 @@
         <v>9070</v>
       </c>
       <c r="F1047548" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G1047548" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1047548" s="18">
         <v>6.7699999999999996E-2</v>
       </c>
       <c r="I1047548" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047548" s="49"/>
     </row>
@@ -34092,10 +34095,10 @@
         <v>6</v>
       </c>
       <c r="F1047549" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G1047549" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="G1047549" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="H1047549" s="18"/>
       <c r="I1047549" s="19"/>
@@ -34106,10 +34109,10 @@
         <v>304</v>
       </c>
       <c r="F1047550" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1047550" s="5" t="s">
         <v>130</v>
-      </c>
-      <c r="G1047550" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="H1047550" s="18"/>
       <c r="I1047550" s="19"/>
@@ -34120,10 +34123,10 @@
         <v>1231</v>
       </c>
       <c r="F1047551" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G1047551" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1047551" s="18"/>
       <c r="I1047551" s="19"/>
@@ -34134,10 +34137,10 @@
         <v>9059</v>
       </c>
       <c r="F1047552" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G1047552" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="G1047552" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="H1047552" s="18"/>
       <c r="I1047552" s="19"/>
@@ -34148,10 +34151,10 @@
         <v>4</v>
       </c>
       <c r="F1047553" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G1047553" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1047553" s="18"/>
       <c r="I1047553" s="19"/>
@@ -34162,10 +34165,10 @@
         <v>9037</v>
       </c>
       <c r="F1047554" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G1047554" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1047554" s="18"/>
       <c r="I1047554" s="19"/>
@@ -34176,16 +34179,16 @@
         <v>1230</v>
       </c>
       <c r="F1047555" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1047555" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="G1047555" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="H1047555" s="18">
         <v>6.7699999999999996E-2</v>
       </c>
       <c r="I1047555" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047555" s="49"/>
     </row>
@@ -34194,10 +34197,10 @@
         <v>108</v>
       </c>
       <c r="F1047556" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1047556" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="G1047556" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="H1047556" s="18"/>
       <c r="I1047556" s="19"/>
@@ -34208,10 +34211,10 @@
         <v>400</v>
       </c>
       <c r="F1047557" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G1047557" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H1047557" s="18"/>
       <c r="I1047557" s="19"/>
@@ -34222,10 +34225,10 @@
         <v>403</v>
       </c>
       <c r="F1047558" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G1047558" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H1047558" s="18"/>
       <c r="I1047558" s="19"/>
@@ -34236,10 +34239,10 @@
         <v>3265</v>
       </c>
       <c r="F1047559" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G1047559" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H1047559" s="18"/>
       <c r="I1047559" s="19"/>
@@ -34250,10 +34253,10 @@
         <v>1617</v>
       </c>
       <c r="F1047560" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G1047560" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H1047560" s="18"/>
       <c r="I1047560" s="19"/>
@@ -34264,16 +34267,16 @@
         <v>1546</v>
       </c>
       <c r="F1047561" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1047561" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="G1047561" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="H1047561" s="18">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I1047561" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047561" s="49"/>
     </row>
@@ -34282,10 +34285,10 @@
         <v>290</v>
       </c>
       <c r="F1047562" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G1047562" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1047562" s="18"/>
       <c r="I1047562" s="19"/>
@@ -34296,10 +34299,10 @@
         <v>9005</v>
       </c>
       <c r="F1047563" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G1047563" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H1047563" s="18"/>
       <c r="I1047563" s="19"/>
@@ -34310,10 +34313,10 @@
         <v>1593</v>
       </c>
       <c r="F1047564" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G1047564" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H1047564" s="18"/>
       <c r="I1047564" s="19"/>
@@ -34324,10 +34327,10 @@
         <v>3308</v>
       </c>
       <c r="F1047565" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G1047565" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1047565" s="18"/>
       <c r="I1047565" s="19"/>
@@ -34338,10 +34341,10 @@
         <v>500</v>
       </c>
       <c r="F1047566" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G1047566" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H1047566" s="18"/>
       <c r="I1047566" s="19"/>
@@ -34352,16 +34355,16 @@
         <v>9061</v>
       </c>
       <c r="F1047567" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G1047567" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H1047567" s="18">
         <v>6.7699999999999996E-2</v>
       </c>
       <c r="I1047567" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047567" s="49"/>
     </row>
@@ -34370,10 +34373,10 @@
         <v>303</v>
       </c>
       <c r="F1047568" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G1047568" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1047568" s="18"/>
       <c r="I1047568" s="19"/>
@@ -34384,10 +34387,10 @@
         <v>95</v>
       </c>
       <c r="F1047569" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G1047569" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H1047569" s="18"/>
       <c r="I1047569" s="19"/>
@@ -34398,10 +34401,10 @@
         <v>8</v>
       </c>
       <c r="F1047570" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G1047570" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H1047570" s="18"/>
       <c r="I1047570" s="19"/>
@@ -34412,10 +34415,10 @@
         <v>20509</v>
       </c>
       <c r="F1047571" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G1047571" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H1047571" s="18"/>
       <c r="I1047571" s="19"/>
@@ -34426,10 +34429,10 @@
         <v>20508</v>
       </c>
       <c r="F1047572" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G1047572" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H1047572" s="18"/>
       <c r="I1047572" s="19"/>
@@ -34440,10 +34443,10 @@
         <v>20525</v>
       </c>
       <c r="F1047573" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G1047573" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H1047573" s="18"/>
       <c r="I1047573" s="19"/>
@@ -34454,10 +34457,10 @@
         <v>20511</v>
       </c>
       <c r="F1047574" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G1047574" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1047574" s="18"/>
       <c r="I1047574" s="19"/>
@@ -34468,10 +34471,10 @@
         <v>20521</v>
       </c>
       <c r="F1047575" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G1047575" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H1047575" s="18"/>
       <c r="I1047575" s="19"/>
@@ -34482,10 +34485,10 @@
         <v>501</v>
       </c>
       <c r="F1047576" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G1047576" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H1047576" s="18"/>
       <c r="I1047576" s="19"/>
@@ -34496,10 +34499,10 @@
         <v>90</v>
       </c>
       <c r="F1047577" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G1047577" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1047577" s="18"/>
       <c r="I1047577" s="19"/>
@@ -34510,10 +34513,10 @@
         <v>106</v>
       </c>
       <c r="F1047578" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1047578" s="5" t="s">
         <v>162</v>
-      </c>
-      <c r="G1047578" s="5" t="s">
-        <v>163</v>
       </c>
       <c r="H1047578" s="18"/>
       <c r="I1047578" s="19"/>
@@ -34524,10 +34527,10 @@
         <v>91</v>
       </c>
       <c r="F1047579" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G1047579" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H1047579" s="18"/>
       <c r="I1047579" s="19"/>
@@ -34538,10 +34541,10 @@
         <v>275</v>
       </c>
       <c r="F1047580" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1047580" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="G1047580" s="5" t="s">
-        <v>166</v>
       </c>
       <c r="H1047580" s="18"/>
       <c r="I1047580" s="19"/>
@@ -34552,16 +34555,16 @@
         <v>9062</v>
       </c>
       <c r="F1047581" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1047581" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="G1047581" s="5" t="s">
-        <v>168</v>
       </c>
       <c r="H1047581" s="18">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="I1047581" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047581" s="49"/>
     </row>
@@ -34570,10 +34573,10 @@
         <v>159</v>
       </c>
       <c r="F1047582" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1047582" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="G1047582" s="5" t="s">
-        <v>170</v>
       </c>
       <c r="H1047582" s="18"/>
       <c r="I1047582" s="19"/>
@@ -34584,10 +34587,10 @@
         <v>99</v>
       </c>
       <c r="F1047583" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G1047583" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1047583" s="18"/>
       <c r="I1047583" s="19"/>
@@ -34598,10 +34601,10 @@
         <v>133</v>
       </c>
       <c r="F1047584" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G1047584" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H1047584" s="18"/>
       <c r="I1047584" s="19"/>
@@ -34612,10 +34615,10 @@
         <v>266</v>
       </c>
       <c r="F1047585" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G1047585" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1047585" s="18"/>
       <c r="I1047585" s="19"/>
@@ -34626,10 +34629,10 @@
         <v>38</v>
       </c>
       <c r="F1047586" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1047586" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="G1047586" s="5" t="s">
-        <v>175</v>
       </c>
       <c r="H1047586" s="18"/>
       <c r="I1047586" s="19"/>
@@ -34640,10 +34643,10 @@
         <v>9</v>
       </c>
       <c r="F1047587" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1047587" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="G1047587" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="H1047587" s="18"/>
       <c r="I1047587" s="19"/>
@@ -34654,16 +34657,16 @@
         <v>16455</v>
       </c>
       <c r="F1047588" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1047588" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="G1047588" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="H1047588" s="18">
         <v>2.75E-2</v>
       </c>
       <c r="I1047588" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047588" s="49"/>
     </row>
@@ -34672,10 +34675,10 @@
         <v>312</v>
       </c>
       <c r="F1047589" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G1047589" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H1047589" s="18"/>
       <c r="I1047589" s="19"/>
@@ -34686,10 +34689,10 @@
         <v>12173</v>
       </c>
       <c r="F1047590" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1047590" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="G1047590" s="5" t="s">
-        <v>182</v>
       </c>
       <c r="H1047590" s="18"/>
       <c r="I1047590" s="19"/>
@@ -34700,10 +34703,10 @@
         <v>1900</v>
       </c>
       <c r="F1047591" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G1047591" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="G1047591" s="5" t="s">
-        <v>184</v>
       </c>
       <c r="H1047591" s="18"/>
       <c r="I1047591" s="19"/>
@@ -34714,10 +34717,10 @@
         <v>54</v>
       </c>
       <c r="F1047592" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1047592" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="G1047592" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="H1047592" s="18"/>
       <c r="I1047592" s="19"/>
@@ -34728,10 +34731,10 @@
         <v>20534</v>
       </c>
       <c r="F1047593" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G1047593" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H1047593" s="18"/>
       <c r="I1047593" s="19"/>
@@ -34742,16 +34745,16 @@
         <v>1017</v>
       </c>
       <c r="F1047594" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G1047594" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1047594" s="18">
         <v>0.14000000000000001</v>
       </c>
       <c r="I1047594" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047594" s="49"/>
     </row>
@@ -34760,16 +34763,16 @@
         <v>9071</v>
       </c>
       <c r="F1047595" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G1047595" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H1047595" s="18">
         <v>6.7699999999999996E-2</v>
       </c>
       <c r="I1047595" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047595" s="49"/>
     </row>
@@ -34778,16 +34781,16 @@
         <v>9072</v>
       </c>
       <c r="F1047596" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G1047596" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1047596" s="18">
         <v>6.7699999999999996E-2</v>
       </c>
       <c r="I1047596" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047596" s="49"/>
     </row>
@@ -34796,16 +34799,16 @@
         <v>16456</v>
       </c>
       <c r="F1047597" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G1047597" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H1047597" s="18">
         <v>2.75E-2</v>
       </c>
       <c r="I1047597" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047597" s="49"/>
     </row>
@@ -34814,10 +34817,10 @@
         <v>440</v>
       </c>
       <c r="F1047598" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G1047598" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H1047598" s="18"/>
       <c r="I1047598" s="19"/>
@@ -34828,10 +34831,10 @@
         <v>441</v>
       </c>
       <c r="F1047599" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G1047599" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1047599" s="18"/>
       <c r="I1047599" s="19"/>
@@ -34842,10 +34845,10 @@
         <v>442</v>
       </c>
       <c r="F1047600" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1047600" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="G1047600" s="5" t="s">
-        <v>199</v>
       </c>
       <c r="H1047600" s="18"/>
       <c r="I1047600" s="19"/>
@@ -34856,16 +34859,16 @@
         <v>4</v>
       </c>
       <c r="F1047601" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G1047601" s="5" t="s">
         <v>200</v>
-      </c>
-      <c r="G1047601" s="5" t="s">
-        <v>201</v>
       </c>
       <c r="H1047601" s="18">
         <v>2.4E-2</v>
       </c>
       <c r="I1047601" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047601" s="49"/>
     </row>
@@ -34874,16 +34877,16 @@
         <v>9037</v>
       </c>
       <c r="F1047602" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G1047602" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H1047602" s="18">
         <v>6.7699999999999996E-2</v>
       </c>
       <c r="I1047602" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J1047602" s="49"/>
     </row>
@@ -34892,10 +34895,10 @@
         <v>1609</v>
       </c>
       <c r="F1047603" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G1047603" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H1047603" s="18"/>
       <c r="I1047603" s="19"/>
@@ -34906,10 +34909,10 @@
         <v>208</v>
       </c>
       <c r="F1047604" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1047604" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="G1047604" s="5" t="s">
-        <v>206</v>
       </c>
       <c r="H1047604" s="18"/>
       <c r="I1047604" s="19"/>
@@ -34920,10 +34923,10 @@
         <v>1805</v>
       </c>
       <c r="F1047605" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G1047605" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="G1047605" s="5" t="s">
-        <v>208</v>
       </c>
       <c r="H1047605" s="18"/>
       <c r="I1047605" s="19"/>
@@ -34934,10 +34937,10 @@
         <v>520</v>
       </c>
       <c r="F1047606" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G1047606" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H1047606" s="18"/>
       <c r="I1047606" s="19"/>
@@ -34948,10 +34951,10 @@
         <v>521</v>
       </c>
       <c r="F1047607" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G1047607" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H1047607" s="18"/>
       <c r="I1047607" s="19"/>
@@ -34962,10 +34965,10 @@
         <v>522</v>
       </c>
       <c r="F1047608" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G1047608" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1047608" s="18"/>
       <c r="I1047608" s="19"/>
@@ -34976,10 +34979,10 @@
         <v>523</v>
       </c>
       <c r="F1047609" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G1047609" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H1047609" s="18"/>
       <c r="I1047609" s="19"/>
@@ -34990,10 +34993,10 @@
         <v>101</v>
       </c>
       <c r="F1047610" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G1047610" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H1047610" s="18"/>
       <c r="I1047610" s="19"/>
@@ -35003,10 +35006,10 @@
         <v>102</v>
       </c>
       <c r="F1047611" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G1047611" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1047611" s="18"/>
       <c r="I1047611" s="19"/>
@@ -35016,10 +35019,10 @@
         <v>526</v>
       </c>
       <c r="F1047612" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1047612" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="G1047612" s="5" t="s">
-        <v>218</v>
       </c>
       <c r="H1047612" s="18"/>
       <c r="I1047612" s="19"/>
@@ -35029,10 +35032,10 @@
         <v>524</v>
       </c>
       <c r="F1047613" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G1047613" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H1047613" s="18"/>
       <c r="I1047613" s="19"/>
@@ -35042,10 +35045,10 @@
         <v>515</v>
       </c>
       <c r="F1047614" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G1047614" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H1047614" s="22"/>
       <c r="I1047614" s="23"/>

</xml_diff>